<commit_message>
Added files + changed epsi
</commit_message>
<xml_diff>
--- a/Figures/satisfaction.xlsx
+++ b/Figures/satisfaction.xlsx
@@ -72,8 +72,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -151,19 +154,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>80.0</c:v>
+                  <c:v>95.86879999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>74.7624</c:v>
+                  <c:v>87.8661</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>71.7893</c:v>
+                  <c:v>64.7206</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>38.3686</c:v>
+                  <c:v>12.1339</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>85.4965</c:v>
+                  <c:v>48.5467</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -177,11 +180,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2134756648"/>
-        <c:axId val="2134734328"/>
+        <c:axId val="2100675032"/>
+        <c:axId val="2080196968"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="2134756648"/>
+        <c:axId val="2100675032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -191,7 +194,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2134734328"/>
+        <c:crossAx val="2080196968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -199,7 +202,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2134734328"/>
+        <c:axId val="2080196968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -210,7 +213,7 @@
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2134756648"/>
+        <c:crossAx val="2100675032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -612,7 +615,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -630,7 +633,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>80</v>
+        <v>95.868799999999993</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -638,7 +641,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>74.7624</v>
+        <v>87.866100000000003</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -646,7 +649,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>71.789299999999997</v>
+        <v>64.720600000000005</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -654,15 +657,15 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>38.368600000000001</v>
+        <v>12.133900000000001</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6">
-        <v>85.496499999999997</v>
+      <c r="B6" s="1">
+        <v>48.546700000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>